<commit_message>
légére optimisation (4% de rapidité) brutForce v4.1
</commit_message>
<xml_diff>
--- a/RéunificationStatistiques.xlsx
+++ b/RéunificationStatistiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Université\Projets\ProjetS3Voyageur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA795FD-E9E6-49AE-99E7-41C5F8FB154E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C364681-E345-492B-B995-D490DAB6A427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4477,8 +4477,8 @@
   <autoFilter ref="A2:O9" xr:uid="{D3A00F70-4E7F-4B97-9C0A-D230A153E3C9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{37C6C5CD-2283-4DA4-8094-2B49747C3015}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{8F038FC7-D535-4ECF-8829-F6E116FE7D6C}" uniqueName="20" name="Colonne2" queryTableFieldId="20" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{AC89F13A-F553-44D6-A213-EDE7D33682A4}" uniqueName="19" name="Colonne1" queryTableFieldId="19" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{8F038FC7-D535-4ECF-8829-F6E116FE7D6C}" uniqueName="20" name="Colonne2" queryTableFieldId="20" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{AC89F13A-F553-44D6-A213-EDE7D33682A4}" uniqueName="19" name="Colonne1" queryTableFieldId="19" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{F860B5AF-5C87-4959-B023-1D01251738A5}" uniqueName="2" name="3" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{52321CB8-2C0E-4C53-8E10-B355604B41CF}" uniqueName="3" name="4" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{1A9257C4-36C3-4655-A6BD-49DBC71EDB5F}" uniqueName="4" name="5" queryTableFieldId="4"/>
@@ -4500,9 +4500,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E4719F83-5FDE-498D-AD89-BE8E90FDBBB7}" name="Stats_1" displayName="Stats_1" ref="A27:O34" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A27:O34" xr:uid="{B8E75324-E23F-4109-9DE2-31D264928AA9}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{5CD28F4E-ADA1-4640-A9AA-4959FEBA80B6}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{5AC6386D-F7E4-4A15-9C0E-A68EC71DC693}" uniqueName="20" name="1" queryTableFieldId="20" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{A13DFDD6-B227-44E4-BBD8-F04862DEDFE9}" uniqueName="19" name="2" queryTableFieldId="19" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5CD28F4E-ADA1-4640-A9AA-4959FEBA80B6}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{5AC6386D-F7E4-4A15-9C0E-A68EC71DC693}" uniqueName="20" name="1" queryTableFieldId="20" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{A13DFDD6-B227-44E4-BBD8-F04862DEDFE9}" uniqueName="19" name="2" queryTableFieldId="19" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6035DBA4-AB3B-4E43-8880-7FE2EE113DB4}" uniqueName="2" name="3" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{081E72E5-883A-461D-BE66-D7B563B2AF06}" uniqueName="3" name="4" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{3E0C540B-02C6-4B9E-8455-FFEACF0A713B}" uniqueName="4" name="5" queryTableFieldId="4"/>
@@ -5357,8 +5357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F4F023-ED55-44A4-A031-89C7FE3816FD}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6310,10 +6310,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Revert "légére optimisation (4% de rapidité) brutForce v4.1"
This reverts commit 1f9eadfca9326449ec3aeee84b43292b6045582a.
</commit_message>
<xml_diff>
--- a/RéunificationStatistiques.xlsx
+++ b/RéunificationStatistiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Université\Projets\ProjetS3Voyageur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C364681-E345-492B-B995-D490DAB6A427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA795FD-E9E6-49AE-99E7-41C5F8FB154E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4477,8 +4477,8 @@
   <autoFilter ref="A2:O9" xr:uid="{D3A00F70-4E7F-4B97-9C0A-D230A153E3C9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{37C6C5CD-2283-4DA4-8094-2B49747C3015}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{8F038FC7-D535-4ECF-8829-F6E116FE7D6C}" uniqueName="20" name="Colonne2" queryTableFieldId="20" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{AC89F13A-F553-44D6-A213-EDE7D33682A4}" uniqueName="19" name="Colonne1" queryTableFieldId="19" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{8F038FC7-D535-4ECF-8829-F6E116FE7D6C}" uniqueName="20" name="Colonne2" queryTableFieldId="20" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{AC89F13A-F553-44D6-A213-EDE7D33682A4}" uniqueName="19" name="Colonne1" queryTableFieldId="19" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{F860B5AF-5C87-4959-B023-1D01251738A5}" uniqueName="2" name="3" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{52321CB8-2C0E-4C53-8E10-B355604B41CF}" uniqueName="3" name="4" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{1A9257C4-36C3-4655-A6BD-49DBC71EDB5F}" uniqueName="4" name="5" queryTableFieldId="4"/>
@@ -4500,9 +4500,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E4719F83-5FDE-498D-AD89-BE8E90FDBBB7}" name="Stats_1" displayName="Stats_1" ref="A27:O34" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A27:O34" xr:uid="{B8E75324-E23F-4109-9DE2-31D264928AA9}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{5CD28F4E-ADA1-4640-A9AA-4959FEBA80B6}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{5AC6386D-F7E4-4A15-9C0E-A68EC71DC693}" uniqueName="20" name="1" queryTableFieldId="20" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{A13DFDD6-B227-44E4-BBD8-F04862DEDFE9}" uniqueName="19" name="2" queryTableFieldId="19" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5CD28F4E-ADA1-4640-A9AA-4959FEBA80B6}" uniqueName="1" name="Algorithmes" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{5AC6386D-F7E4-4A15-9C0E-A68EC71DC693}" uniqueName="20" name="1" queryTableFieldId="20" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{A13DFDD6-B227-44E4-BBD8-F04862DEDFE9}" uniqueName="19" name="2" queryTableFieldId="19" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{6035DBA4-AB3B-4E43-8880-7FE2EE113DB4}" uniqueName="2" name="3" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{081E72E5-883A-461D-BE66-D7B563B2AF06}" uniqueName="3" name="4" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{3E0C540B-02C6-4B9E-8455-FFEACF0A713B}" uniqueName="4" name="5" queryTableFieldId="4"/>
@@ -5357,8 +5357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F4F023-ED55-44A4-A031-89C7FE3816FD}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:O26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6310,6 +6310,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="2">

</xml_diff>